<commit_message>
Created a line graph to filter by countries but having issues combining information from rankings.xls and scraped data
</commit_message>
<xml_diff>
--- a/FSI_output.xlsx
+++ b/FSI_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E180"/>
+  <dimension ref="A1:D180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,17 +441,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>FSI Total</t>
+          <t>Total</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>FSI Total Normalized</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>FSI Total Normalized x4</t>
+          <t>Year</t>
         </is>
       </c>
     </row>
@@ -468,10 +463,7 @@
         <v>111.3</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>4</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="3">
@@ -487,10 +479,7 @@
         <v>109.3</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9797160243407708</v>
-      </c>
-      <c r="E3" t="n">
-        <v>3.918864097363083</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="4">
@@ -506,10 +495,7 @@
         <v>109</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9766734279918864</v>
-      </c>
-      <c r="E4" t="n">
-        <v>3.906693711967546</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="5">
@@ -525,10 +511,7 @@
         <v>108.1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9675456389452333</v>
-      </c>
-      <c r="E5" t="n">
-        <v>3.870182555780933</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="6">
@@ -544,10 +527,7 @@
         <v>106.7</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9533468559837729</v>
-      </c>
-      <c r="E6" t="n">
-        <v>3.813387423935092</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="7">
@@ -563,10 +543,7 @@
         <v>106.6</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9523326572008113</v>
-      </c>
-      <c r="E7" t="n">
-        <v>3.809330628803245</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="8">
@@ -582,10 +559,7 @@
         <v>103.9</v>
       </c>
       <c r="D8" t="n">
-        <v>0.924949290060852</v>
-      </c>
-      <c r="E8" t="n">
-        <v>3.699797160243408</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="9">
@@ -601,10 +575,7 @@
         <v>103.9</v>
       </c>
       <c r="D9" t="n">
-        <v>0.924949290060852</v>
-      </c>
-      <c r="E9" t="n">
-        <v>3.699797160243408</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="10">
@@ -620,10 +591,7 @@
         <v>103.5</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9208924949290062</v>
-      </c>
-      <c r="E10" t="n">
-        <v>3.683569979716025</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="11">
@@ -639,10 +607,7 @@
         <v>102.7</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9127789046653144</v>
-      </c>
-      <c r="E11" t="n">
-        <v>3.651115618661258</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="12">
@@ -658,10 +623,7 @@
         <v>100</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8853955375253549</v>
-      </c>
-      <c r="E12" t="n">
-        <v>3.54158215010142</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="13">
@@ -677,10 +639,7 @@
         <v>98.09999999999999</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8661257606490872</v>
-      </c>
-      <c r="E13" t="n">
-        <v>3.464503042596349</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="14">
@@ -696,10 +655,7 @@
         <v>97.8</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8630831643002028</v>
-      </c>
-      <c r="E14" t="n">
-        <v>3.452332657200811</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="15">
@@ -715,10 +671,7 @@
         <v>97.3</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8580121703853956</v>
-      </c>
-      <c r="E15" t="n">
-        <v>3.432048681541582</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="16">
@@ -734,10 +687,7 @@
         <v>96.59999999999999</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8509127789046653</v>
-      </c>
-      <c r="E16" t="n">
-        <v>3.403651115618661</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="17">
@@ -753,10 +703,7 @@
         <v>96.5</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8498985801217038</v>
-      </c>
-      <c r="E17" t="n">
-        <v>3.399594320486815</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="18">
@@ -772,10 +719,7 @@
         <v>96.40000000000001</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8488843813387424</v>
-      </c>
-      <c r="E18" t="n">
-        <v>3.39553752535497</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="19">
@@ -791,10 +735,7 @@
         <v>95.7</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8417849898580122</v>
-      </c>
-      <c r="E19" t="n">
-        <v>3.367139959432049</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="20">
@@ -810,10 +751,7 @@
         <v>95.2</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8367139959432049</v>
-      </c>
-      <c r="E20" t="n">
-        <v>3.34685598377282</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="21">
@@ -829,10 +767,7 @@
         <v>94.3</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8275862068965517</v>
-      </c>
-      <c r="E21" t="n">
-        <v>3.310344827586207</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="22">
@@ -848,10 +783,7 @@
         <v>94.2</v>
       </c>
       <c r="D22" t="n">
-        <v>0.8265720081135903</v>
-      </c>
-      <c r="E22" t="n">
-        <v>3.306288032454361</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="23">
@@ -867,10 +799,7 @@
         <v>93.09999999999999</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8154158215010141</v>
-      </c>
-      <c r="E23" t="n">
-        <v>3.261663286004056</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="24">
@@ -886,10 +815,7 @@
         <v>92.7</v>
       </c>
       <c r="D24" t="n">
-        <v>0.8113590263691685</v>
-      </c>
-      <c r="E24" t="n">
-        <v>3.245436105476674</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="25">
@@ -905,10 +831,7 @@
         <v>92.59999999999999</v>
       </c>
       <c r="D25" t="n">
-        <v>0.8103448275862069</v>
-      </c>
-      <c r="E25" t="n">
-        <v>3.241379310344827</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="26">
@@ -924,10 +847,7 @@
         <v>92.5</v>
       </c>
       <c r="D26" t="n">
-        <v>0.8093306288032455</v>
-      </c>
-      <c r="E26" t="n">
-        <v>3.237322515212982</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="27">
@@ -943,10 +863,7 @@
         <v>92.09999999999999</v>
       </c>
       <c r="D27" t="n">
-        <v>0.8052738336713996</v>
-      </c>
-      <c r="E27" t="n">
-        <v>3.221095334685598</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="28">
@@ -962,10 +879,7 @@
         <v>91.7</v>
       </c>
       <c r="D28" t="n">
-        <v>0.8012170385395538</v>
-      </c>
-      <c r="E28" t="n">
-        <v>3.204868154158215</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="29">
@@ -981,10 +895,7 @@
         <v>91.09999999999999</v>
       </c>
       <c r="D29" t="n">
-        <v>0.795131845841785</v>
-      </c>
-      <c r="E29" t="n">
-        <v>3.18052738336714</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="30">
@@ -1000,10 +911,7 @@
         <v>90.2</v>
       </c>
       <c r="D30" t="n">
-        <v>0.7860040567951319</v>
-      </c>
-      <c r="E30" t="n">
-        <v>3.144016227180527</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="31">
@@ -1019,10 +927,7 @@
         <v>89</v>
       </c>
       <c r="D31" t="n">
-        <v>0.7738336713995944</v>
-      </c>
-      <c r="E31" t="n">
-        <v>3.095334685598377</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="32">
@@ -1038,10 +943,7 @@
         <v>88.59999999999999</v>
       </c>
       <c r="D32" t="n">
-        <v>0.7697768762677485</v>
-      </c>
-      <c r="E32" t="n">
-        <v>3.079107505070994</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="33">
@@ -1057,10 +959,7 @@
         <v>88.40000000000001</v>
       </c>
       <c r="D33" t="n">
-        <v>0.7677484787018256</v>
-      </c>
-      <c r="E33" t="n">
-        <v>3.070993914807302</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="34">
@@ -1076,10 +975,7 @@
         <v>88.2</v>
       </c>
       <c r="D34" t="n">
-        <v>0.7657200811359027</v>
-      </c>
-      <c r="E34" t="n">
-        <v>3.062880324543611</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="35">
@@ -1095,10 +991,7 @@
         <v>87</v>
       </c>
       <c r="D35" t="n">
-        <v>0.7535496957403651</v>
-      </c>
-      <c r="E35" t="n">
-        <v>3.01419878296146</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="36">
@@ -1114,10 +1007,7 @@
         <v>86.90000000000001</v>
       </c>
       <c r="D36" t="n">
-        <v>0.7525354969574037</v>
-      </c>
-      <c r="E36" t="n">
-        <v>3.010141987829615</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="37">
@@ -1133,10 +1023,7 @@
         <v>86.5</v>
       </c>
       <c r="D37" t="n">
-        <v>0.7484787018255579</v>
-      </c>
-      <c r="E37" t="n">
-        <v>2.993914807302231</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="38">
@@ -1152,10 +1039,7 @@
         <v>85.90000000000001</v>
       </c>
       <c r="D38" t="n">
-        <v>0.7423935091277891</v>
-      </c>
-      <c r="E38" t="n">
-        <v>2.969574036511156</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="39">
@@ -1171,10 +1055,7 @@
         <v>85.59999999999999</v>
       </c>
       <c r="D39" t="n">
-        <v>0.7393509127789046</v>
-      </c>
-      <c r="E39" t="n">
-        <v>2.957403651115619</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="40">
@@ -1190,10 +1071,7 @@
         <v>85.3</v>
       </c>
       <c r="D40" t="n">
-        <v>0.7363083164300203</v>
-      </c>
-      <c r="E40" t="n">
-        <v>2.945233265720081</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="41">
@@ -1209,10 +1087,7 @@
         <v>84.90000000000001</v>
       </c>
       <c r="D41" t="n">
-        <v>0.7322515212981745</v>
-      </c>
-      <c r="E41" t="n">
-        <v>2.929006085192698</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="42">
@@ -1228,10 +1103,7 @@
         <v>84</v>
       </c>
       <c r="D42" t="n">
-        <v>0.7231237322515213</v>
-      </c>
-      <c r="E42" t="n">
-        <v>2.892494929006085</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="43">
@@ -1247,10 +1119,7 @@
         <v>83.7</v>
       </c>
       <c r="D43" t="n">
-        <v>0.720081135902637</v>
-      </c>
-      <c r="E43" t="n">
-        <v>2.880324543610548</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="44">
@@ -1266,10 +1135,7 @@
         <v>82.90000000000001</v>
       </c>
       <c r="D44" t="n">
-        <v>0.7119675456389453</v>
-      </c>
-      <c r="E44" t="n">
-        <v>2.847870182555781</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="45">
@@ -1285,10 +1151,7 @@
         <v>82.8</v>
       </c>
       <c r="D45" t="n">
-        <v>0.7109533468559838</v>
-      </c>
-      <c r="E45" t="n">
-        <v>2.843813387423935</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="46">
@@ -1304,10 +1167,7 @@
         <v>82.59999999999999</v>
       </c>
       <c r="D46" t="n">
-        <v>0.7089249492900608</v>
-      </c>
-      <c r="E46" t="n">
-        <v>2.835699797160243</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="47">
@@ -1323,10 +1183,7 @@
         <v>81.8</v>
       </c>
       <c r="D47" t="n">
-        <v>0.7008113590263692</v>
-      </c>
-      <c r="E47" t="n">
-        <v>2.803245436105477</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="48">
@@ -1342,10 +1199,7 @@
         <v>81.7</v>
       </c>
       <c r="D48" t="n">
-        <v>0.6997971602434078</v>
-      </c>
-      <c r="E48" t="n">
-        <v>2.799188640973631</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="49">
@@ -1361,10 +1215,7 @@
         <v>81.59999999999999</v>
       </c>
       <c r="D49" t="n">
-        <v>0.6987829614604462</v>
-      </c>
-      <c r="E49" t="n">
-        <v>2.795131845841785</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="50">
@@ -1380,10 +1231,7 @@
         <v>81.59999999999999</v>
       </c>
       <c r="D50" t="n">
-        <v>0.6987829614604462</v>
-      </c>
-      <c r="E50" t="n">
-        <v>2.795131845841785</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="51">
@@ -1399,10 +1247,7 @@
         <v>81.2</v>
       </c>
       <c r="D51" t="n">
-        <v>0.6947261663286004</v>
-      </c>
-      <c r="E51" t="n">
-        <v>2.778904665314402</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="52">
@@ -1418,10 +1263,7 @@
         <v>81.09999999999999</v>
       </c>
       <c r="D52" t="n">
-        <v>0.6937119675456389</v>
-      </c>
-      <c r="E52" t="n">
-        <v>2.774847870182556</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="53">
@@ -1437,10 +1279,7 @@
         <v>80.5</v>
       </c>
       <c r="D53" t="n">
-        <v>0.6876267748478702</v>
-      </c>
-      <c r="E53" t="n">
-        <v>2.750507099391481</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="54">
@@ -1456,10 +1295,7 @@
         <v>79.8</v>
       </c>
       <c r="D54" t="n">
-        <v>0.6805273833671399</v>
-      </c>
-      <c r="E54" t="n">
-        <v>2.72210953346856</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="55">
@@ -1475,10 +1311,7 @@
         <v>78.8</v>
       </c>
       <c r="D55" t="n">
-        <v>0.6703853955375253</v>
-      </c>
-      <c r="E55" t="n">
-        <v>2.681541582150101</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="56">
@@ -1494,10 +1327,7 @@
         <v>78.59999999999999</v>
       </c>
       <c r="D56" t="n">
-        <v>0.6683569979716024</v>
-      </c>
-      <c r="E56" t="n">
-        <v>2.67342799188641</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="57">
@@ -1513,10 +1343,7 @@
         <v>78.09999999999999</v>
       </c>
       <c r="D57" t="n">
-        <v>0.6632860040567951</v>
-      </c>
-      <c r="E57" t="n">
-        <v>2.65314401622718</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="58">
@@ -1532,10 +1359,7 @@
         <v>78</v>
       </c>
       <c r="D58" t="n">
-        <v>0.6622718052738337</v>
-      </c>
-      <c r="E58" t="n">
-        <v>2.649087221095335</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="59">
@@ -1551,10 +1375,7 @@
         <v>77.59999999999999</v>
       </c>
       <c r="D59" t="n">
-        <v>0.6582150101419878</v>
-      </c>
-      <c r="E59" t="n">
-        <v>2.632860040567951</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="60">
@@ -1570,10 +1391,7 @@
         <v>77.59999999999999</v>
       </c>
       <c r="D60" t="n">
-        <v>0.6582150101419878</v>
-      </c>
-      <c r="E60" t="n">
-        <v>2.632860040567951</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="61">
@@ -1589,10 +1407,7 @@
         <v>76.7</v>
       </c>
       <c r="D61" t="n">
-        <v>0.6490872210953347</v>
-      </c>
-      <c r="E61" t="n">
-        <v>2.596348884381339</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="62">
@@ -1608,10 +1423,7 @@
         <v>76.09999999999999</v>
       </c>
       <c r="D62" t="n">
-        <v>0.6430020283975659</v>
-      </c>
-      <c r="E62" t="n">
-        <v>2.572008113590264</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="63">
@@ -1627,10 +1439,7 @@
         <v>75.7</v>
       </c>
       <c r="D63" t="n">
-        <v>0.6389452332657202</v>
-      </c>
-      <c r="E63" t="n">
-        <v>2.555780933062881</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="64">
@@ -1646,10 +1455,7 @@
         <v>75.59999999999999</v>
       </c>
       <c r="D64" t="n">
-        <v>0.6379310344827586</v>
-      </c>
-      <c r="E64" t="n">
-        <v>2.551724137931034</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="65">
@@ -1665,10 +1471,7 @@
         <v>75.09999999999999</v>
       </c>
       <c r="D65" t="n">
-        <v>0.6328600405679513</v>
-      </c>
-      <c r="E65" t="n">
-        <v>2.531440162271805</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="66">
@@ -1684,10 +1487,7 @@
         <v>74.90000000000001</v>
       </c>
       <c r="D66" t="n">
-        <v>0.6308316430020284</v>
-      </c>
-      <c r="E66" t="n">
-        <v>2.523326572008114</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="67">
@@ -1703,10 +1503,7 @@
         <v>74.90000000000001</v>
       </c>
       <c r="D67" t="n">
-        <v>0.6308316430020284</v>
-      </c>
-      <c r="E67" t="n">
-        <v>2.523326572008114</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="68">
@@ -1722,10 +1519,7 @@
         <v>74.8</v>
       </c>
       <c r="D68" t="n">
-        <v>0.6298174442190669</v>
-      </c>
-      <c r="E68" t="n">
-        <v>2.519269776876268</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="69">
@@ -1741,10 +1535,7 @@
         <v>74.59999999999999</v>
       </c>
       <c r="D69" t="n">
-        <v>0.6277890466531439</v>
-      </c>
-      <c r="E69" t="n">
-        <v>2.511156186612576</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="70">
@@ -1760,10 +1551,7 @@
         <v>74.3</v>
       </c>
       <c r="D70" t="n">
-        <v>0.6247464503042596</v>
-      </c>
-      <c r="E70" t="n">
-        <v>2.498985801217038</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="71">
@@ -1779,10 +1567,7 @@
         <v>74.2</v>
       </c>
       <c r="D71" t="n">
-        <v>0.6237322515212982</v>
-      </c>
-      <c r="E71" t="n">
-        <v>2.494929006085193</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="72">
@@ -1798,10 +1583,7 @@
         <v>73.8</v>
       </c>
       <c r="D72" t="n">
-        <v>0.6196754563894523</v>
-      </c>
-      <c r="E72" t="n">
-        <v>2.478701825557809</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="73">
@@ -1817,10 +1599,7 @@
         <v>72.8</v>
       </c>
       <c r="D73" t="n">
-        <v>0.6095334685598377</v>
-      </c>
-      <c r="E73" t="n">
-        <v>2.438133874239351</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="74">
@@ -1836,10 +1615,7 @@
         <v>72.8</v>
       </c>
       <c r="D74" t="n">
-        <v>0.6095334685598377</v>
-      </c>
-      <c r="E74" t="n">
-        <v>2.438133874239351</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="75">
@@ -1855,10 +1631,7 @@
         <v>72.5</v>
       </c>
       <c r="D75" t="n">
-        <v>0.6064908722109533</v>
-      </c>
-      <c r="E75" t="n">
-        <v>2.425963488843813</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="76">
@@ -1874,10 +1647,7 @@
         <v>72.3</v>
       </c>
       <c r="D76" t="n">
-        <v>0.6044624746450304</v>
-      </c>
-      <c r="E76" t="n">
-        <v>2.417849898580122</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="77">
@@ -1893,10 +1663,7 @@
         <v>72</v>
       </c>
       <c r="D77" t="n">
-        <v>0.6014198782961461</v>
-      </c>
-      <c r="E77" t="n">
-        <v>2.405679513184584</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="78">
@@ -1912,10 +1679,7 @@
         <v>71</v>
       </c>
       <c r="D78" t="n">
-        <v>0.5912778904665315</v>
-      </c>
-      <c r="E78" t="n">
-        <v>2.365111561866126</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="79">
@@ -1931,10 +1695,7 @@
         <v>70.3</v>
       </c>
       <c r="D79" t="n">
-        <v>0.5841784989858012</v>
-      </c>
-      <c r="E79" t="n">
-        <v>2.336713995943205</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="80">
@@ -1950,10 +1711,7 @@
         <v>70.2</v>
       </c>
       <c r="D80" t="n">
-        <v>0.5831643002028398</v>
-      </c>
-      <c r="E80" t="n">
-        <v>2.332657200811359</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="81">
@@ -1969,10 +1727,7 @@
         <v>69.59999999999999</v>
       </c>
       <c r="D81" t="n">
-        <v>0.577079107505071</v>
-      </c>
-      <c r="E81" t="n">
-        <v>2.308316430020284</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="82">
@@ -1988,10 +1743,7 @@
         <v>69.40000000000001</v>
       </c>
       <c r="D82" t="n">
-        <v>0.5750507099391481</v>
-      </c>
-      <c r="E82" t="n">
-        <v>2.300202839756592</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="83">
@@ -2007,10 +1759,7 @@
         <v>69.3</v>
       </c>
       <c r="D83" t="n">
-        <v>0.5740365111561866</v>
-      </c>
-      <c r="E83" t="n">
-        <v>2.296146044624746</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="84">
@@ -2026,10 +1775,7 @@
         <v>69</v>
       </c>
       <c r="D84" t="n">
-        <v>0.5709939148073022</v>
-      </c>
-      <c r="E84" t="n">
-        <v>2.283975659229209</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="85">
@@ -2045,10 +1791,7 @@
         <v>68.8</v>
       </c>
       <c r="D85" t="n">
-        <v>0.5689655172413793</v>
-      </c>
-      <c r="E85" t="n">
-        <v>2.275862068965517</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="86">
@@ -2064,10 +1807,7 @@
         <v>68.7</v>
       </c>
       <c r="D86" t="n">
-        <v>0.5679513184584178</v>
-      </c>
-      <c r="E86" t="n">
-        <v>2.271805273833671</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="87">
@@ -2083,10 +1823,7 @@
         <v>68.7</v>
       </c>
       <c r="D87" t="n">
-        <v>0.5679513184584178</v>
-      </c>
-      <c r="E87" t="n">
-        <v>2.271805273833671</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="88">
@@ -2102,10 +1839,7 @@
         <v>68.59999999999999</v>
       </c>
       <c r="D88" t="n">
-        <v>0.5669371196754563</v>
-      </c>
-      <c r="E88" t="n">
-        <v>2.267748478701825</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="89">
@@ -2121,10 +1855,7 @@
         <v>68.5</v>
       </c>
       <c r="D89" t="n">
-        <v>0.565922920892495</v>
-      </c>
-      <c r="E89" t="n">
-        <v>2.26369168356998</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="90">
@@ -2140,10 +1871,7 @@
         <v>68.09999999999999</v>
       </c>
       <c r="D90" t="n">
-        <v>0.561866125760649</v>
-      </c>
-      <c r="E90" t="n">
-        <v>2.247464503042596</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="91">
@@ -2159,10 +1887,7 @@
         <v>68</v>
       </c>
       <c r="D91" t="n">
-        <v>0.5608519269776876</v>
-      </c>
-      <c r="E91" t="n">
-        <v>2.24340770791075</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="92">
@@ -2178,10 +1903,7 @@
         <v>67.8</v>
       </c>
       <c r="D92" t="n">
-        <v>0.5588235294117647</v>
-      </c>
-      <c r="E92" t="n">
-        <v>2.235294117647059</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="93">
@@ -2197,10 +1919,7 @@
         <v>67.2</v>
       </c>
       <c r="D93" t="n">
-        <v>0.552738336713996</v>
-      </c>
-      <c r="E93" t="n">
-        <v>2.210953346855984</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="94">
@@ -2216,10 +1935,7 @@
         <v>66.90000000000001</v>
       </c>
       <c r="D94" t="n">
-        <v>0.5496957403651116</v>
-      </c>
-      <c r="E94" t="n">
-        <v>2.198782961460446</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="95">
@@ -2235,10 +1951,7 @@
         <v>66.40000000000001</v>
       </c>
       <c r="D95" t="n">
-        <v>0.5446247464503043</v>
-      </c>
-      <c r="E95" t="n">
-        <v>2.178498985801217</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="96">
@@ -2254,10 +1967,7 @@
         <v>66.2</v>
       </c>
       <c r="D96" t="n">
-        <v>0.5425963488843814</v>
-      </c>
-      <c r="E96" t="n">
-        <v>2.170385395537525</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="97">
@@ -2273,10 +1983,7 @@
         <v>64.8</v>
       </c>
       <c r="D97" t="n">
-        <v>0.5283975659229209</v>
-      </c>
-      <c r="E97" t="n">
-        <v>2.113590263691683</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="98">
@@ -2292,10 +1999,7 @@
         <v>64.7</v>
       </c>
       <c r="D98" t="n">
-        <v>0.5273833671399595</v>
-      </c>
-      <c r="E98" t="n">
-        <v>2.109533468559838</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="99">
@@ -2311,10 +2015,7 @@
         <v>64.5</v>
       </c>
       <c r="D99" t="n">
-        <v>0.5253549695740365</v>
-      </c>
-      <c r="E99" t="n">
-        <v>2.101419878296146</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="100">
@@ -2330,10 +2031,7 @@
         <v>64.40000000000001</v>
       </c>
       <c r="D100" t="n">
-        <v>0.5243407707910751</v>
-      </c>
-      <c r="E100" t="n">
-        <v>2.0973630831643</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="101">
@@ -2349,10 +2047,7 @@
         <v>64.2</v>
       </c>
       <c r="D101" t="n">
-        <v>0.5223123732251521</v>
-      </c>
-      <c r="E101" t="n">
-        <v>2.089249492900608</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="102">
@@ -2368,10 +2063,7 @@
         <v>63.9</v>
       </c>
       <c r="D102" t="n">
-        <v>0.5192697768762679</v>
-      </c>
-      <c r="E102" t="n">
-        <v>2.077079107505071</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="103">
@@ -2387,10 +2079,7 @@
         <v>63.7</v>
       </c>
       <c r="D103" t="n">
-        <v>0.5172413793103449</v>
-      </c>
-      <c r="E103" t="n">
-        <v>2.068965517241379</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="104">
@@ -2406,10 +2095,7 @@
         <v>63.2</v>
       </c>
       <c r="D104" t="n">
-        <v>0.5121703853955376</v>
-      </c>
-      <c r="E104" t="n">
-        <v>2.04868154158215</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="105">
@@ -2425,10 +2111,7 @@
         <v>62.2</v>
       </c>
       <c r="D105" t="n">
-        <v>0.502028397565923</v>
-      </c>
-      <c r="E105" t="n">
-        <v>2.008113590263692</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="106">
@@ -2444,10 +2127,7 @@
         <v>61.5</v>
       </c>
       <c r="D106" t="n">
-        <v>0.4949290060851927</v>
-      </c>
-      <c r="E106" t="n">
-        <v>1.979716024340771</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="107">
@@ -2463,10 +2143,7 @@
         <v>60.8</v>
       </c>
       <c r="D107" t="n">
-        <v>0.4878296146044624</v>
-      </c>
-      <c r="E107" t="n">
-        <v>1.95131845841785</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="108">
@@ -2482,10 +2159,7 @@
         <v>60.3</v>
       </c>
       <c r="D108" t="n">
-        <v>0.4827586206896551</v>
-      </c>
-      <c r="E108" t="n">
-        <v>1.931034482758621</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="109">
@@ -2501,10 +2175,7 @@
         <v>60.2</v>
       </c>
       <c r="D109" t="n">
-        <v>0.4817444219066938</v>
-      </c>
-      <c r="E109" t="n">
-        <v>1.926977687626775</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="110">
@@ -2520,10 +2191,7 @@
         <v>59.3</v>
       </c>
       <c r="D110" t="n">
-        <v>0.4726166328600405</v>
-      </c>
-      <c r="E110" t="n">
-        <v>1.890466531440162</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="111">
@@ -2539,10 +2207,7 @@
         <v>59.3</v>
       </c>
       <c r="D111" t="n">
-        <v>0.4726166328600405</v>
-      </c>
-      <c r="E111" t="n">
-        <v>1.890466531440162</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="112">
@@ -2558,10 +2223,7 @@
         <v>59.2</v>
       </c>
       <c r="D112" t="n">
-        <v>0.4716024340770791</v>
-      </c>
-      <c r="E112" t="n">
-        <v>1.886409736308317</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="113">
@@ -2577,10 +2239,7 @@
         <v>59.1</v>
       </c>
       <c r="D113" t="n">
-        <v>0.4705882352941178</v>
-      </c>
-      <c r="E113" t="n">
-        <v>1.882352941176471</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="114">
@@ -2596,10 +2255,7 @@
         <v>58.8</v>
       </c>
       <c r="D114" t="n">
-        <v>0.4675456389452332</v>
-      </c>
-      <c r="E114" t="n">
-        <v>1.870182555780933</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="115">
@@ -2615,10 +2271,7 @@
         <v>58.1</v>
       </c>
       <c r="D115" t="n">
-        <v>0.4604462474645031</v>
-      </c>
-      <c r="E115" t="n">
-        <v>1.841784989858013</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="116">
@@ -2634,10 +2287,7 @@
         <v>57.8</v>
       </c>
       <c r="D116" t="n">
-        <v>0.4574036511156186</v>
-      </c>
-      <c r="E116" t="n">
-        <v>1.829614604462475</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="117">
@@ -2653,10 +2303,7 @@
         <v>57.2</v>
       </c>
       <c r="D117" t="n">
-        <v>0.4513184584178499</v>
-      </c>
-      <c r="E117" t="n">
-        <v>1.8052738336714</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="118">
@@ -2672,10 +2319,7 @@
         <v>57</v>
       </c>
       <c r="D118" t="n">
-        <v>0.449290060851927</v>
-      </c>
-      <c r="E118" t="n">
-        <v>1.797160243407708</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="119">
@@ -2691,10 +2335,7 @@
         <v>56.9</v>
       </c>
       <c r="D119" t="n">
-        <v>0.4482758620689656</v>
-      </c>
-      <c r="E119" t="n">
-        <v>1.793103448275862</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="120">
@@ -2710,10 +2351,7 @@
         <v>56.2</v>
       </c>
       <c r="D120" t="n">
-        <v>0.4411764705882353</v>
-      </c>
-      <c r="E120" t="n">
-        <v>1.764705882352941</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="121">
@@ -2729,10 +2367,7 @@
         <v>55.9</v>
       </c>
       <c r="D121" t="n">
-        <v>0.438133874239351</v>
-      </c>
-      <c r="E121" t="n">
-        <v>1.752535496957404</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="122">
@@ -2748,10 +2383,7 @@
         <v>54.7</v>
       </c>
       <c r="D122" t="n">
-        <v>0.4259634888438134</v>
-      </c>
-      <c r="E122" t="n">
-        <v>1.703853955375254</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="123">
@@ -2767,10 +2399,7 @@
         <v>54.1</v>
       </c>
       <c r="D123" t="n">
-        <v>0.4198782961460447</v>
-      </c>
-      <c r="E123" t="n">
-        <v>1.679513184584179</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="124">
@@ -2786,10 +2415,7 @@
         <v>53.9</v>
       </c>
       <c r="D124" t="n">
-        <v>0.4178498985801218</v>
-      </c>
-      <c r="E124" t="n">
-        <v>1.671399594320487</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="125">
@@ -2805,10 +2431,7 @@
         <v>53.6</v>
       </c>
       <c r="D125" t="n">
-        <v>0.4148073022312374</v>
-      </c>
-      <c r="E125" t="n">
-        <v>1.65922920892495</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="126">
@@ -2824,10 +2447,7 @@
         <v>53.5</v>
       </c>
       <c r="D126" t="n">
-        <v>0.4137931034482759</v>
-      </c>
-      <c r="E126" t="n">
-        <v>1.655172413793103</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="127">
@@ -2843,10 +2463,7 @@
         <v>53.1</v>
       </c>
       <c r="D127" t="n">
-        <v>0.4097363083164301</v>
-      </c>
-      <c r="E127" t="n">
-        <v>1.63894523326572</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="128">
@@ -2862,10 +2479,7 @@
         <v>51.9</v>
       </c>
       <c r="D128" t="n">
-        <v>0.3975659229208925</v>
-      </c>
-      <c r="E128" t="n">
-        <v>1.59026369168357</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="129">
@@ -2881,10 +2495,7 @@
         <v>51.9</v>
       </c>
       <c r="D129" t="n">
-        <v>0.3975659229208925</v>
-      </c>
-      <c r="E129" t="n">
-        <v>1.59026369168357</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="130">
@@ -2900,10 +2511,7 @@
         <v>51.5</v>
       </c>
       <c r="D130" t="n">
-        <v>0.3935091277890466</v>
-      </c>
-      <c r="E130" t="n">
-        <v>1.574036511156186</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="131">
@@ -2919,10 +2527,7 @@
         <v>51</v>
       </c>
       <c r="D131" t="n">
-        <v>0.3884381338742394</v>
-      </c>
-      <c r="E131" t="n">
-        <v>1.553752535496957</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="132">
@@ -2938,10 +2543,7 @@
         <v>51</v>
       </c>
       <c r="D132" t="n">
-        <v>0.3884381338742394</v>
-      </c>
-      <c r="E132" t="n">
-        <v>1.553752535496957</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="133">
@@ -2957,10 +2559,7 @@
         <v>50.7</v>
       </c>
       <c r="D133" t="n">
-        <v>0.385395537525355</v>
-      </c>
-      <c r="E133" t="n">
-        <v>1.54158215010142</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="134">
@@ -2976,10 +2575,7 @@
         <v>49.4</v>
       </c>
       <c r="D134" t="n">
-        <v>0.3722109533468561</v>
-      </c>
-      <c r="E134" t="n">
-        <v>1.488843813387424</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="135">
@@ -2995,10 +2591,7 @@
         <v>49.3</v>
       </c>
       <c r="D135" t="n">
-        <v>0.3711967545638945</v>
-      </c>
-      <c r="E135" t="n">
-        <v>1.484787018255578</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="136">
@@ -3014,10 +2607,7 @@
         <v>48</v>
       </c>
       <c r="D136" t="n">
-        <v>0.3580121703853955</v>
-      </c>
-      <c r="E136" t="n">
-        <v>1.432048681541582</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="137">
@@ -3033,10 +2623,7 @@
         <v>47.7</v>
       </c>
       <c r="D137" t="n">
-        <v>0.3549695740365112</v>
-      </c>
-      <c r="E137" t="n">
-        <v>1.419878296146045</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="138">
@@ -3052,10 +2639,7 @@
         <v>47.4</v>
       </c>
       <c r="D138" t="n">
-        <v>0.3519269776876268</v>
-      </c>
-      <c r="E138" t="n">
-        <v>1.407707910750507</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="139">
@@ -3071,10 +2655,7 @@
         <v>46.2</v>
       </c>
       <c r="D139" t="n">
-        <v>0.3397565922920893</v>
-      </c>
-      <c r="E139" t="n">
-        <v>1.359026369168357</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="140">
@@ -3090,10 +2671,7 @@
         <v>45.9</v>
       </c>
       <c r="D140" t="n">
-        <v>0.3367139959432049</v>
-      </c>
-      <c r="E140" t="n">
-        <v>1.34685598377282</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="141">
@@ -3109,10 +2687,7 @@
         <v>44.7</v>
       </c>
       <c r="D141" t="n">
-        <v>0.3245436105476673</v>
-      </c>
-      <c r="E141" t="n">
-        <v>1.298174442190669</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="142">
@@ -3128,10 +2703,7 @@
         <v>44.5</v>
       </c>
       <c r="D142" t="n">
-        <v>0.3225152129817445</v>
-      </c>
-      <c r="E142" t="n">
-        <v>1.290060851926978</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="143">
@@ -3147,10 +2719,7 @@
         <v>44.2</v>
       </c>
       <c r="D143" t="n">
-        <v>0.3194726166328601</v>
-      </c>
-      <c r="E143" t="n">
-        <v>1.27789046653144</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="144">
@@ -3166,10 +2735,7 @@
         <v>44</v>
       </c>
       <c r="D144" t="n">
-        <v>0.3174442190669371</v>
-      </c>
-      <c r="E144" t="n">
-        <v>1.269776876267749</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="145">
@@ -3185,10 +2751,7 @@
         <v>41.7</v>
       </c>
       <c r="D145" t="n">
-        <v>0.2941176470588236</v>
-      </c>
-      <c r="E145" t="n">
-        <v>1.176470588235294</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="146">
@@ -3204,10 +2767,7 @@
         <v>41.4</v>
       </c>
       <c r="D146" t="n">
-        <v>0.2910750507099392</v>
-      </c>
-      <c r="E146" t="n">
-        <v>1.164300202839757</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="147">
@@ -3223,10 +2783,7 @@
         <v>41.1</v>
       </c>
       <c r="D147" t="n">
-        <v>0.2880324543610548</v>
-      </c>
-      <c r="E147" t="n">
-        <v>1.152129817444219</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="148">
@@ -3242,10 +2799,7 @@
         <v>41.1</v>
       </c>
       <c r="D148" t="n">
-        <v>0.2880324543610548</v>
-      </c>
-      <c r="E148" t="n">
-        <v>1.152129817444219</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="149">
@@ -3261,10 +2815,7 @@
         <v>40.8</v>
       </c>
       <c r="D149" t="n">
-        <v>0.2849898580121704</v>
-      </c>
-      <c r="E149" t="n">
-        <v>1.139959432048681</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="150">
@@ -3280,10 +2831,7 @@
         <v>39.8</v>
       </c>
       <c r="D150" t="n">
-        <v>0.2748478701825558</v>
-      </c>
-      <c r="E150" t="n">
-        <v>1.099391480730223</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="151">
@@ -3299,10 +2847,7 @@
         <v>39.4</v>
       </c>
       <c r="D151" t="n">
-        <v>0.2707910750507099</v>
-      </c>
-      <c r="E151" t="n">
-        <v>1.08316430020284</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="152">
@@ -3318,10 +2863,7 @@
         <v>37.8</v>
       </c>
       <c r="D152" t="n">
-        <v>0.2545638945233266</v>
-      </c>
-      <c r="E152" t="n">
-        <v>1.018255578093306</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="153">
@@ -3337,10 +2879,7 @@
         <v>37.7</v>
       </c>
       <c r="D153" t="n">
-        <v>0.2535496957403652</v>
-      </c>
-      <c r="E153" t="n">
-        <v>1.014198782961461</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="154">
@@ -3356,10 +2895,7 @@
         <v>37.4</v>
       </c>
       <c r="D154" t="n">
-        <v>0.2505070993914807</v>
-      </c>
-      <c r="E154" t="n">
-        <v>1.002028397565923</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="155">
@@ -3375,10 +2911,7 @@
         <v>36.5</v>
       </c>
       <c r="D155" t="n">
-        <v>0.2413793103448276</v>
-      </c>
-      <c r="E155" t="n">
-        <v>0.9655172413793104</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="156">
@@ -3394,10 +2927,7 @@
         <v>35.3</v>
       </c>
       <c r="D156" t="n">
-        <v>0.22920892494929</v>
-      </c>
-      <c r="E156" t="n">
-        <v>0.9168356997971602</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="157">
@@ -3413,10 +2943,7 @@
         <v>34.7</v>
       </c>
       <c r="D157" t="n">
-        <v>0.2231237322515214</v>
-      </c>
-      <c r="E157" t="n">
-        <v>0.8924949290060854</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="158">
@@ -3432,10 +2959,7 @@
         <v>33.7</v>
       </c>
       <c r="D158" t="n">
-        <v>0.2129817444219067</v>
-      </c>
-      <c r="E158" t="n">
-        <v>0.8519269776876269</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="159">
@@ -3451,10 +2975,7 @@
         <v>31.1</v>
       </c>
       <c r="D159" t="n">
-        <v>0.1866125760649087</v>
-      </c>
-      <c r="E159" t="n">
-        <v>0.746450304259635</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="160">
@@ -3470,10 +2991,7 @@
         <v>30.3</v>
       </c>
       <c r="D160" t="n">
-        <v>0.1784989858012171</v>
-      </c>
-      <c r="E160" t="n">
-        <v>0.7139959432048683</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="161">
@@ -3489,10 +3007,7 @@
         <v>30.2</v>
       </c>
       <c r="D161" t="n">
-        <v>0.1774847870182556</v>
-      </c>
-      <c r="E161" t="n">
-        <v>0.7099391480730224</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="162">
@@ -3508,10 +3023,7 @@
         <v>29.8</v>
       </c>
       <c r="D162" t="n">
-        <v>0.1734279918864098</v>
-      </c>
-      <c r="E162" t="n">
-        <v>0.693711967545639</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="163">
@@ -3527,10 +3039,7 @@
         <v>28.3</v>
       </c>
       <c r="D163" t="n">
-        <v>0.1582150101419879</v>
-      </c>
-      <c r="E163" t="n">
-        <v>0.6328600405679514</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="164">
@@ -3546,10 +3055,7 @@
         <v>26.1</v>
       </c>
       <c r="D164" t="n">
-        <v>0.1359026369168357</v>
-      </c>
-      <c r="E164" t="n">
-        <v>0.543610547667343</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="165">
@@ -3565,10 +3071,7 @@
         <v>25.9</v>
       </c>
       <c r="D165" t="n">
-        <v>0.1338742393509128</v>
-      </c>
-      <c r="E165" t="n">
-        <v>0.5354969574036511</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="166">
@@ -3584,10 +3087,7 @@
         <v>25.4</v>
       </c>
       <c r="D166" t="n">
-        <v>0.1288032454361055</v>
-      </c>
-      <c r="E166" t="n">
-        <v>0.5152129817444219</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="167">
@@ -3603,10 +3103,7 @@
         <v>24</v>
       </c>
       <c r="D167" t="n">
-        <v>0.114604462474645</v>
-      </c>
-      <c r="E167" t="n">
-        <v>0.4584178498985802</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="168">
@@ -3622,10 +3119,7 @@
         <v>23.1</v>
       </c>
       <c r="D168" t="n">
-        <v>0.1054766734279919</v>
-      </c>
-      <c r="E168" t="n">
-        <v>0.4219066937119677</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="169">
@@ -3641,10 +3135,7 @@
         <v>20.6</v>
       </c>
       <c r="D169" t="n">
-        <v>0.08012170385395539</v>
-      </c>
-      <c r="E169" t="n">
-        <v>0.3204868154158216</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="170">
@@ -3660,10 +3151,7 @@
         <v>19.6</v>
       </c>
       <c r="D170" t="n">
-        <v>0.06997971602434079</v>
-      </c>
-      <c r="E170" t="n">
-        <v>0.2799188640973632</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="171">
@@ -3679,10 +3167,7 @@
         <v>19.5</v>
       </c>
       <c r="D171" t="n">
-        <v>0.06896551724137932</v>
-      </c>
-      <c r="E171" t="n">
-        <v>0.2758620689655173</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="172">
@@ -3698,10 +3183,7 @@
         <v>18.7</v>
       </c>
       <c r="D172" t="n">
-        <v>0.06085192697768763</v>
-      </c>
-      <c r="E172" t="n">
-        <v>0.2434077079107505</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="173">
@@ -3717,10 +3199,7 @@
         <v>18.6</v>
       </c>
       <c r="D173" t="n">
-        <v>0.05983772819472619</v>
-      </c>
-      <c r="E173" t="n">
-        <v>0.2393509127789048</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="174">
@@ -3736,10 +3215,7 @@
         <v>18.6</v>
       </c>
       <c r="D174" t="n">
-        <v>0.05983772819472619</v>
-      </c>
-      <c r="E174" t="n">
-        <v>0.2393509127789048</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="175">
@@ -3755,10 +3231,7 @@
         <v>16.2</v>
       </c>
       <c r="D175" t="n">
-        <v>0.03549695740365112</v>
-      </c>
-      <c r="E175" t="n">
-        <v>0.1419878296146045</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="176">
@@ -3774,10 +3247,7 @@
         <v>15.9</v>
       </c>
       <c r="D176" t="n">
-        <v>0.03245436105476675</v>
-      </c>
-      <c r="E176" t="n">
-        <v>0.129817444219067</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="177">
@@ -3793,10 +3263,7 @@
         <v>15.9</v>
       </c>
       <c r="D177" t="n">
-        <v>0.03245436105476675</v>
-      </c>
-      <c r="E177" t="n">
-        <v>0.129817444219067</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="178">
@@ -3812,10 +3279,7 @@
         <v>15.2</v>
       </c>
       <c r="D178" t="n">
-        <v>0.02535496957403651</v>
-      </c>
-      <c r="E178" t="n">
-        <v>0.1014198782961461</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="179">
@@ -3831,10 +3295,7 @@
         <v>14.3</v>
       </c>
       <c r="D179" t="n">
-        <v>0.01622718052738338</v>
-      </c>
-      <c r="E179" t="n">
-        <v>0.06490872210953352</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="180">
@@ -3850,10 +3311,7 @@
         <v>12.7</v>
       </c>
       <c r="D180" t="n">
-        <v>0</v>
-      </c>
-      <c r="E180" t="n">
-        <v>0</v>
+        <v>2024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>